<commit_message>
HoanT2 : null check order
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/国民年金第３号被保険者住所変更届.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/国民年金第３号被保険者住所変更届.xlsx
@@ -833,16 +833,16 @@
     <t>電　　　　　　話</t>
   </si>
   <si>
-    <t xml:space="preserve">      短期在留　　   住民票住所以外の居所　
-      海外居住           その他（　　　　　　　　　                     ）</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 ９</t>
   </si>
   <si>
-    <t xml:space="preserve">     短期在留　　         住民票住所以外の居所　
-     海外居住             その他（　　　　　　　　                   ）  </t>
+    <t xml:space="preserve">     短期在留　　          住民票住所以外の居所　
+     海外居住              その他（　　　　　　　　                   ）  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      短期在留　　       住民票住所以外の居所　
+      海外居住           その他（　　　　　　　　　                     ）</t>
   </si>
 </sst>
 </file>
@@ -6680,16 +6680,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>12</xdr:col>
+          <xdr:col>14</xdr:col>
           <xdr:colOff>95250</xdr:colOff>
-          <xdr:row>17</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>15</xdr:col>
+          <xdr:col>17</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -8058,16 +8058,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>145446</xdr:rowOff>
+      <xdr:rowOff>174021</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8082,7 +8082,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1876425" y="3876675"/>
+          <a:off x="2124075" y="3905250"/>
           <a:ext cx="152400" cy="154971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8452,6 +8452,44 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>114275</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>371332</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="82" name="Picture 81"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3914775" y="6677025"/>
+          <a:ext cx="200000" cy="1142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8757,8 +8795,8 @@
   </sheetPr>
   <dimension ref="C1:CX75"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="BT29" sqref="BT29"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="17.25" customHeight="1"/>
@@ -9713,7 +9751,7 @@
       <c r="AH14" s="168"/>
       <c r="AI14" s="168"/>
       <c r="AJ14" s="181" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="AK14" s="182"/>
       <c r="AL14" s="182"/>
@@ -10391,7 +10429,7 @@
       <c r="BO24" s="93"/>
       <c r="BP24" s="94"/>
       <c r="BQ24" s="99" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BR24" s="100"/>
       <c r="BS24" s="122"/>
@@ -10650,7 +10688,7 @@
       <c r="BK27" s="231"/>
       <c r="BL27" s="232"/>
       <c r="BM27" s="236" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BN27" s="237"/>
       <c r="BO27" s="237"/>
@@ -11656,16 +11694,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>12</xdr:col>
+                    <xdr:col>14</xdr:col>
                     <xdr:colOff>95250</xdr:colOff>
-                    <xdr:row>17</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>15</xdr:col>
+                    <xdr:col>17</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>18</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
hoant2: fix bug family dummy code
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/国民年金第３号被保険者住所変更届.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/国民年金第３号被保険者住所変更届.xlsx
@@ -841,8 +841,8 @@
     <t>　　　　　　　　　　　     （         被保険者と配偶者は同居している。）</t>
   </si>
   <si>
-    <t xml:space="preserve">      短期在留　　          住民票住所以外の居所　
-      海外居住              その他（　　　　                   ）  </t>
+    <t xml:space="preserve">        短期在留　　           住民票住所以外の居所　
+        海外居住                      その他（　　　                   ）  </t>
   </si>
 </sst>
 </file>
@@ -7278,16 +7278,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>50</xdr:col>
-      <xdr:colOff>66676</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>190501</xdr:rowOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>21851</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>64</xdr:col>
-      <xdr:colOff>85726</xdr:colOff>
+      <xdr:col>70</xdr:col>
+      <xdr:colOff>100853</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:rowOff>156882</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7302,8 +7302,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6543676" y="3114676"/>
-          <a:ext cx="1752600" cy="171450"/>
+          <a:off x="6353175" y="3148854"/>
+          <a:ext cx="2701178" cy="156881"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7735,14 +7735,14 @@
     <xdr:from>
       <xdr:col>42</xdr:col>
       <xdr:colOff>114301</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>168089</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
+      <xdr:colOff>33618</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>183546</xdr:rowOff>
+      <xdr:rowOff>183547</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7757,8 +7757,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5600701" y="3152775"/>
-          <a:ext cx="152400" cy="154971"/>
+          <a:off x="5582772" y="3115236"/>
+          <a:ext cx="165846" cy="217164"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7994,15 +7994,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>70</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>39781</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>71</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>68356</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>183546</xdr:rowOff>
+      <xdr:rowOff>183547</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8017,8 +8017,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9010650" y="5715000"/>
-          <a:ext cx="152400" cy="154971"/>
+          <a:off x="8993281" y="5754782"/>
+          <a:ext cx="151840" cy="154971"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8123,16 +8123,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>74</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
+      <xdr:col>76</xdr:col>
+      <xdr:colOff>112058</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:rowOff>33617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>82</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>95</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
+      <xdr:rowOff>201706</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8147,8 +8147,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9563099" y="5734051"/>
-          <a:ext cx="1019176" cy="180974"/>
+          <a:off x="9805146" y="5759823"/>
+          <a:ext cx="2286001" cy="168089"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8327,14 +8327,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>80</xdr:col>
-      <xdr:colOff>59221</xdr:colOff>
+      <xdr:col>81</xdr:col>
+      <xdr:colOff>3191</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>83</xdr:col>
-      <xdr:colOff>106846</xdr:colOff>
+      <xdr:col>84</xdr:col>
+      <xdr:colOff>50816</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
@@ -8345,8 +8345,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10304808" y="5449957"/>
-          <a:ext cx="420342" cy="235641"/>
+          <a:off x="10312603" y="5513294"/>
+          <a:ext cx="417419" cy="241488"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8462,8 +8462,8 @@
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>114275</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>371332</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>1538</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8834,7 +8834,7 @@
   <dimension ref="C1:CX75"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:BG4"/>
+      <selection activeCell="S7" sqref="S7:W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="17.25" customHeight="1"/>
@@ -9172,11 +9172,11 @@
       <c r="P7" s="104"/>
       <c r="Q7" s="105"/>
       <c r="R7" s="104"/>
-      <c r="S7" s="36"/>
-      <c r="T7" s="83"/>
-      <c r="U7" s="83"/>
-      <c r="V7" s="83"/>
-      <c r="W7" s="83"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
       <c r="X7" s="36"/>
       <c r="Y7" s="37"/>
       <c r="Z7" s="46"/>
@@ -9257,11 +9257,11 @@
       <c r="P8" s="104"/>
       <c r="Q8" s="105"/>
       <c r="R8" s="104"/>
-      <c r="S8" s="38"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="34"/>
-      <c r="V8" s="34"/>
-      <c r="W8" s="34"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="44"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="44"/>
+      <c r="W8" s="44"/>
       <c r="X8" s="38"/>
       <c r="Y8" s="35"/>
       <c r="Z8" s="48"/>

</xml_diff>

<commit_message>
record không đòng nhất
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/国民年金第３号被保険者住所変更届.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/国民年金第３号被保険者住所変更届.xlsx
@@ -842,7 +842,7 @@
   </si>
   <si>
     <t xml:space="preserve">      短期在留　　           住民票住所以外の居所　
-      海外居住                     その他（　　　                      ）  </t>
+      海外居住               その他（　　                      ）  </t>
   </si>
 </sst>
 </file>
@@ -2949,8 +2949,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
-          <a:off x="580551" y="205154"/>
-          <a:ext cx="2218592" cy="935704"/>
+          <a:off x="573730" y="205154"/>
+          <a:ext cx="2235157" cy="912318"/>
           <a:chOff x="0" y="0"/>
           <a:chExt cx="227" cy="85"/>
         </a:xfrm>
@@ -6748,13 +6748,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>63</xdr:col>
-          <xdr:colOff>97491</xdr:colOff>
+          <xdr:colOff>95250</xdr:colOff>
           <xdr:row>26</xdr:row>
           <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>66</xdr:col>
-          <xdr:colOff>31376</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
@@ -6815,13 +6815,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>63</xdr:col>
-          <xdr:colOff>97491</xdr:colOff>
+          <xdr:colOff>95250</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>66</xdr:col>
-          <xdr:colOff>31376</xdr:colOff>
+          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>27</xdr:row>
           <xdr:rowOff>228600</xdr:rowOff>
         </xdr:to>
@@ -8124,15 +8124,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>75</xdr:col>
-      <xdr:colOff>67235</xdr:colOff>
+      <xdr:colOff>58953</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>22413</xdr:rowOff>
+      <xdr:rowOff>14130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>86</xdr:col>
-      <xdr:colOff>67236</xdr:colOff>
+      <xdr:colOff>58954</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>212912</xdr:rowOff>
+      <xdr:rowOff>204629</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8147,8 +8147,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9637059" y="5748619"/>
-          <a:ext cx="1355912" cy="190499"/>
+          <a:off x="9683344" y="5671152"/>
+          <a:ext cx="1366632" cy="190499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8474,14 +8474,14 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>194225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>114275</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>1538</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>341123</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -8498,8 +8498,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3914775" y="6677025"/>
-          <a:ext cx="200000" cy="1142857"/>
+          <a:off x="3922643" y="6613247"/>
+          <a:ext cx="200415" cy="1140811"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8851,8 +8851,8 @@
   </sheetPr>
   <dimension ref="C1:CX75"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="BN29" sqref="BN29"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" view="pageBreakPreview" topLeftCell="N14" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="BS29" activeCellId="1" sqref="BM27:CF28 BS29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.625" defaultRowHeight="17.25" customHeight="1"/>

</xml_diff>